<commit_message>
mayor update: handsontable auto complete + rekap sppd
</commit_message>
<xml_diff>
--- a/template/HonorTemplate.xlsx
+++ b/template/HonorTemplate.xlsx
@@ -2417,18 +2417,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B120:E120"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B90:E90"/>
+    <mergeCell ref="B91:E91"/>
+    <mergeCell ref="B119:E119"/>
     <mergeCell ref="B33:E33"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B120:E120"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="B90:E90"/>
-    <mergeCell ref="B91:E91"/>
-    <mergeCell ref="B119:E119"/>
   </mergeCells>
   <pageMargins left="0.47" right="0.32" top="0.77" bottom="0.63" header="0.32" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>